<commit_message>
Updated BOM list and added new items
</commit_message>
<xml_diff>
--- a/Dokumentation/EksamensProjekt_Fog - Skruer og tilbehør.xlsx
+++ b/Dokumentation/EksamensProjekt_Fog - Skruer og tilbehør.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\google drive\Datamatiker\2_semester\Eksamensprojekt\Kode\Materialer-Skruer-Tilbehør\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\google drive\Datamatiker\2_semester\Eksamensprojekt\Kode\Dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCD92BD6-75E0-4024-9926-AA9DA5889989}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72266908-A6FB-4527-8F05-960773566026}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="83">
   <si>
     <t>Tilbehør til spær:</t>
   </si>
@@ -253,6 +253,27 @@
   </si>
   <si>
     <t>Pris pr. enhed</t>
+  </si>
+  <si>
+    <t>Tag</t>
+  </si>
+  <si>
+    <t>20,4 x 23,6</t>
+  </si>
+  <si>
+    <t>20,4 x 23,6 tagsten "Gammel dansk"</t>
+  </si>
+  <si>
+    <t>109 x 240</t>
+  </si>
+  <si>
+    <t>109 x 240 Trapez tagplade</t>
+  </si>
+  <si>
+    <t>19x100</t>
+  </si>
+  <si>
+    <t>19x100 Beklædning af skur</t>
   </si>
 </sst>
 </file>
@@ -669,10 +690,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AC51"/>
+  <dimension ref="A1:AC56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1508,9 +1529,87 @@
         <v>49.95</v>
       </c>
     </row>
+    <row r="52" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B52" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="C52" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="D52" s="19">
+        <v>1</v>
+      </c>
+      <c r="E52" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="F52" s="7">
+        <v>9.9499999999999993</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="6"/>
+      <c r="B53" s="4"/>
+      <c r="C53" s="4"/>
+      <c r="D53" s="6"/>
+      <c r="E53" s="6"/>
+      <c r="F53" s="7"/>
+    </row>
+    <row r="54" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="6"/>
+      <c r="B54" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="C54" s="4"/>
+      <c r="D54" s="6"/>
+      <c r="E54" s="6"/>
+      <c r="F54" s="7"/>
+    </row>
+    <row r="55" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B55" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="C55" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="D55" s="6">
+        <v>1</v>
+      </c>
+      <c r="E55" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="F55" s="7">
+        <v>17.95</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B56" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C56" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="D56" s="6">
+        <v>1</v>
+      </c>
+      <c r="E56" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="F56" s="7">
+        <v>84.95</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A87" xr:uid="{8DA8D44F-D07F-4199-9E15-76D61EAE3BB0}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A88" xr:uid="{8DA8D44F-D07F-4199-9E15-76D61EAE3BB0}">
       <formula1>tagtyper</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
CarportCalc kan nu vælge den rigtige spærafstand automatisk
</commit_message>
<xml_diff>
--- a/Dokumentation/EksamensProjekt_Fog - Skruer og tilbehør.xlsx
+++ b/Dokumentation/EksamensProjekt_Fog - Skruer og tilbehør.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\google drive\Datamatiker\2_semester\Eksamensprojekt\Kode\Dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72266908-A6FB-4527-8F05-960773566026}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB76EC00-A577-4974-AA49-A8B584E99C95}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -412,7 +412,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -472,6 +472,7 @@
     <xf numFmtId="164" fontId="12" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -690,10 +691,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AC56"/>
+  <dimension ref="A1:AC57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A56" sqref="A56"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1491,7 +1492,7 @@
     </row>
     <row r="50" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="6" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B50" s="11" t="s">
         <v>54</v>
@@ -1606,6 +1607,9 @@
       <c r="F56" s="7">
         <v>84.95</v>
       </c>
+    </row>
+    <row r="57" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B57" s="27"/>
     </row>
   </sheetData>
   <dataValidations count="1">

</xml_diff>